<commit_message>
KiCad FS error + updated BOM
</commit_message>
<xml_diff>
--- a/KiCAD/APEDSK-AU-BOM.xlsx
+++ b/KiCAD/APEDSK-AU-BOM.xlsx
@@ -29,18 +29,12 @@
     <t>1N5711</t>
   </si>
   <si>
-    <t>5.1K</t>
-  </si>
-  <si>
     <t>330R</t>
   </si>
   <si>
     <t>74LS245</t>
   </si>
   <si>
-    <t>74LS541</t>
-  </si>
-  <si>
     <t>74HC595</t>
   </si>
   <si>
@@ -53,15 +47,9 @@
     <t>Refercence</t>
   </si>
   <si>
-    <t>Schottky; 1N4148 etc works as well</t>
-  </si>
-  <si>
     <t>Industrial Card Edge Slot Socket Connector 22x2P 44P 2.54mm 0.1" 3A * 240-44</t>
   </si>
   <si>
-    <t>Arduino stackable header pack</t>
-  </si>
-  <si>
     <t>R1-R3</t>
   </si>
   <si>
@@ -119,16 +107,28 @@
     <t>74HCT245 should work as well (not tested)</t>
   </si>
   <si>
-    <t>74HCT541 works as well</t>
-  </si>
-  <si>
-    <t>74HCT595 should work as well (not tested)</t>
-  </si>
-  <si>
     <t>IS61C512-20M</t>
   </si>
   <si>
     <t>GAL16V8</t>
+  </si>
+  <si>
+    <t>Schottky; 1N4148 should work as well</t>
+  </si>
+  <si>
+    <t>Arduino stackable header pack (long version)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.1K</t>
+  </si>
+  <si>
+    <t>74HCT541</t>
+  </si>
+  <si>
+    <t>74LS541 should work as well</t>
+  </si>
+  <si>
+    <t>any reasonably close value should work fine (i.e. 4.7K)</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,24 +491,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
         <v>7</v>
@@ -516,10 +516,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -536,81 +536,84 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
       </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -618,38 +621,38 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -657,24 +660,21 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>

</xml_diff>